<commit_message>
ADMIN PAGE BIJNA COMPLETE!!!!!!!!
>>update organism afgewerkt,
>>insert organism werkt nu ook zonder foto,
>>subfamily insert en update aangemaakt
>> season = DONE!
>>select all organism aangepast >> enkel gevalideerde items weergeven
(voor dashboard.jsp)
>>ajax file opgeruimd en gesorteerd per function type
>> forms sluiten automatisch af + geven melding hiervan
>> errormessages werken bij diegene waarbij ze nog niet werkten
>> forms worden pas leeggemaakt na close call (gebruiker hoeft geen
blanco fields te zien na succesvol te updaten/inserten)
>>en nog iets maar dat ben ik al vergeten :-)

TODO:
errormessages komen er dubbel in na insert/updaten = fix??!
ddl in update forms > jquery.focus() werkt niet, misschien proberen om
via index te werken?
--------
Ik neem bovenstaande todo's wel op.
</commit_message>
<xml_diff>
--- a/Doc/Logboeken/Eric_Log.xlsx
+++ b/Doc/Logboeken/Eric_Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -86,10 +86,16 @@
     <t>Code Dal + bugfixes + multipartconfig in ajax</t>
   </si>
   <si>
-    <t>0-02-2015</t>
-  </si>
-  <si>
     <t>multipartconfig in ajax</t>
+  </si>
+  <si>
+    <t>Update organism, errorhandling, dal</t>
+  </si>
+  <si>
+    <t>ajax, error, ddl vs jQuery research, subfamily fix, code</t>
+  </si>
+  <si>
+    <t>10 uur</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,14 +544,36 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
+      <c r="A11" s="2">
+        <v>42036</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>42065</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LOG + required fields fix (dashboard.jsp)
</commit_message>
<xml_diff>
--- a/Doc/Logboeken/Eric_Log.xlsx
+++ b/Doc/Logboeken/Eric_Log.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>datum</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>13-02-215</t>
+  </si>
+  <si>
+    <t>validation on all input fields + various fixes</t>
+  </si>
+  <si>
+    <t>display dynamic photo on all forms + various fixes</t>
+  </si>
+  <si>
+    <t>confirm messages + delete functions + required fields + detailpage + refactoring</t>
+  </si>
+  <si>
+    <t>13 uur</t>
   </si>
 </sst>
 </file>
@@ -209,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,9 +283,22 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -945,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -976,277 +1001,304 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21">
+      <c r="A3" s="24">
         <v>42044</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
+      <c r="A4" s="24">
         <v>42046</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21">
+      <c r="A6" s="24">
         <v>42048</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
+      <c r="A7" s="24">
         <v>42056</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21">
+      <c r="A8" s="24">
         <v>42059</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21">
+      <c r="A9" s="24">
         <v>42061</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21">
+      <c r="A10" s="24">
         <v>42062</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="21">
+      <c r="A11" s="24">
         <v>42063</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="21">
+      <c r="A12" s="24">
         <v>42036</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
+      <c r="A13" s="24">
         <v>42036</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
+      <c r="A14" s="24">
         <v>42065</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="21">
+      <c r="A15" s="24">
         <v>42066</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="21">
+      <c r="A16" s="24">
         <v>42067</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="10"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="10"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="26">
+        <v>42068</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="26">
+        <v>42069</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.15">
+      <c r="A19" s="26">
+        <v>42070</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>

</xml_diff>